<commit_message>
Added some Tuesday Speeches
</commit_message>
<xml_diff>
--- a/DNC/dnc.metadata.xlsx
+++ b/DNC/dnc.metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/DNC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifer/Desktop/Working/2016NCtranscripts/DNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16D2DDB0-0E72-B346-B362-50D0932BAD8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727460E1-7D87-EA4D-8E17-523D779B6424}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Last</t>
   </si>
@@ -124,6 +124,36 @@
   </si>
   <si>
     <t>dnc.obamamichelle.txt</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>Astrid</t>
+  </si>
+  <si>
+    <t>dnc.silva.txt</t>
+  </si>
+  <si>
+    <t>Harkin</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>dnc.harkin.txt</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Grimes</t>
+  </si>
+  <si>
+    <t>Alison</t>
+  </si>
+  <si>
+    <t>dnc.grimes.txt</t>
   </si>
 </sst>
 </file>
@@ -475,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2281F6A-A008-DE4E-A860-242E1F7D7978}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,6 +669,57 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added some RNC speeches
</commit_message>
<xml_diff>
--- a/DNC/dnc.metadata.xlsx
+++ b/DNC/dnc.metadata.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifer/Desktop/Working/2016NCtranscripts/DNC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/DNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727460E1-7D87-EA4D-8E17-523D779B6424}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD91964A-39A9-1E40-A426-F55CF5B60CED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="11240" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Monday" sheetId="1" r:id="rId1"/>
+    <sheet name="Tuesday" sheetId="2" r:id="rId2"/>
+    <sheet name="Wednesday" sheetId="3" r:id="rId3"/>
+    <sheet name="Thursday" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>Last</t>
   </si>
@@ -505,10 +508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2281F6A-A008-DE4E-A860-242E1F7D7978}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,38 +690,138 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B00C89-5F5B-B54D-834C-45D0C98C9369}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D2" t="s">
         <v>37</v>
       </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C4212-161F-404C-AC20-375466C438FF}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D883BCCB-1427-F54B-B447-B53E8EA23A3A}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Key Thursday Speeches
</commit_message>
<xml_diff>
--- a/DNC/dnc.metadata.xlsx
+++ b/DNC/dnc.metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/DNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD91964A-39A9-1E40-A426-F55CF5B60CED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD0F847-9F74-8044-A3F0-3E941EB8F648}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="11240" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="3" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>Last</t>
   </si>
@@ -157,13 +157,40 @@
   </si>
   <si>
     <t>dnc.grimes.txt</t>
+  </si>
+  <si>
+    <t>Clinton</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>dnc.clintonchelsea.txt</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Hillary</t>
+  </si>
+  <si>
+    <t>dnc.clintonhillary.txt</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>Khizer</t>
+  </si>
+  <si>
+    <t>dnc.khan.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -510,17 +537,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2281F6A-A008-DE4E-A860-242E1F7D7978}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="200" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -554,7 +581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -571,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -588,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -605,7 +632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -622,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -639,7 +666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -656,7 +683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -673,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -705,9 +732,9 @@
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -741,7 +768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -772,9 +799,9 @@
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -798,16 +825,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D883BCCB-1427-F54B-B447-B53E8EA23A3A}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -822,6 +852,57 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Tuesday speeches from Cision
</commit_message>
<xml_diff>
--- a/DNC/dnc.metadata.xlsx
+++ b/DNC/dnc.metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/DNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0DE517-0E55-E746-94D3-028C817D2CD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0943CA0E-BB84-4542-A34D-4D79E9DB87E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="3" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="1" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="195">
   <si>
     <t>Last</t>
   </si>
@@ -283,6 +283,342 @@
   </si>
   <si>
     <t>ABC</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Sherman</t>
+  </si>
+  <si>
+    <t>dnc.jacksonsherman.txt</t>
+  </si>
+  <si>
+    <t>Mikulski</t>
+  </si>
+  <si>
+    <t>Barbara</t>
+  </si>
+  <si>
+    <t>dnc.mikulski.txt</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>dnc.lewis.txt</t>
+  </si>
+  <si>
+    <t>Amaru</t>
+  </si>
+  <si>
+    <t>Na'liah</t>
+  </si>
+  <si>
+    <t>dnc.amaru.txt</t>
+  </si>
+  <si>
+    <t>McAuliffe</t>
+  </si>
+  <si>
+    <t>Terry</t>
+  </si>
+  <si>
+    <t>dnc.mcauliffe.txt</t>
+  </si>
+  <si>
+    <t>Gabbard</t>
+  </si>
+  <si>
+    <t>Tulsi</t>
+  </si>
+  <si>
+    <t>dnc.gabbard.txt</t>
+  </si>
+  <si>
+    <t>dnc.housewomen.txt</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>dnc.carterjason.txt</t>
+  </si>
+  <si>
+    <t>Schumer</t>
+  </si>
+  <si>
+    <t>Chuck</t>
+  </si>
+  <si>
+    <t>dnc.schumer.txt</t>
+  </si>
+  <si>
+    <t>Banks</t>
+  </si>
+  <si>
+    <t>dnc.banks.txt</t>
+  </si>
+  <si>
+    <t>Desmond</t>
+  </si>
+  <si>
+    <t>haddeus</t>
+  </si>
+  <si>
+    <t>dnc.desmond.txt</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>Anton</t>
+  </si>
+  <si>
+    <t>dnc.moore.txt</t>
+  </si>
+  <si>
+    <t>Haubert</t>
+  </si>
+  <si>
+    <t>Dynah</t>
+  </si>
+  <si>
+    <t>dnc.haubert.txt</t>
+  </si>
+  <si>
+    <t>Burdick</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>dnc.burdick.txt</t>
+  </si>
+  <si>
+    <t>Parson</t>
+  </si>
+  <si>
+    <t>Dustin</t>
+  </si>
+  <si>
+    <t>dnc.parson.txt</t>
+  </si>
+  <si>
+    <t>Danielle</t>
+  </si>
+  <si>
+    <t>Mellott</t>
+  </si>
+  <si>
+    <t>dnc.mellott.txt</t>
+  </si>
+  <si>
+    <t>Freeman</t>
+  </si>
+  <si>
+    <t>Jelani</t>
+  </si>
+  <si>
+    <t>dnc.freeman.txt</t>
+  </si>
+  <si>
+    <t>Feeney</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>dnc.feeney.txt</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Shyla</t>
+  </si>
+  <si>
+    <t>dnc.nelsonshyla.txt</t>
+  </si>
+  <si>
+    <t>Brazile</t>
+  </si>
+  <si>
+    <t>Donna</t>
+  </si>
+  <si>
+    <t>dnc.brazile.txt</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>dnc.banksdavid.txt</t>
+  </si>
+  <si>
+    <t>Holder</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>dnc.holder.txt</t>
+  </si>
+  <si>
+    <t>Goldwyn</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>dnc.goldwyn.txt</t>
+  </si>
+  <si>
+    <t>Movement</t>
+  </si>
+  <si>
+    <t>Mothers</t>
+  </si>
+  <si>
+    <t>dnc.movement.txt</t>
+  </si>
+  <si>
+    <t>Richards</t>
+  </si>
+  <si>
+    <t>Cecile</t>
+  </si>
+  <si>
+    <t>dnc.richards.txt</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>dnc.benjamin.txt</t>
+  </si>
+  <si>
+    <t>Boxer</t>
+  </si>
+  <si>
+    <t>dnc.boxer.txt</t>
+  </si>
+  <si>
+    <t>Messing</t>
+  </si>
+  <si>
+    <t>Debra</t>
+  </si>
+  <si>
+    <t>dnc.messing.txt</t>
+  </si>
+  <si>
+    <t>Sweeney</t>
+  </si>
+  <si>
+    <t>dnc.sweeney.txt</t>
+  </si>
+  <si>
+    <t>Manning</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>dnc.manning.txt</t>
+  </si>
+  <si>
+    <t>McLay</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>dnc.mclay.txt</t>
+  </si>
+  <si>
+    <t>Crowley</t>
+  </si>
+  <si>
+    <t>dnc.crowley.txt</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Erika</t>
+  </si>
+  <si>
+    <t>dnc.alexander.txt</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>dnc.mooreryan.txt</t>
+  </si>
+  <si>
+    <t>Fererra</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>dnc.fererra.txt</t>
+  </si>
+  <si>
+    <t>Dean</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>dnc.deanhoward.txt</t>
+  </si>
+  <si>
+    <t>Klobuchar</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>dnc.klobuchar.txt</t>
+  </si>
+  <si>
+    <t>Matul</t>
+  </si>
+  <si>
+    <t>Ima</t>
+  </si>
+  <si>
+    <t>dnc.matul.txt</t>
+  </si>
+  <si>
+    <t>Campolo</t>
+  </si>
+  <si>
+    <t>dnc.campolo.txt</t>
+  </si>
+  <si>
+    <t>benediction</t>
+  </si>
+  <si>
+    <t>cision</t>
   </si>
 </sst>
 </file>
@@ -855,19 +1191,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B00C89-5F5B-B54D-834C-45D0C98C9369}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -887,7 +1223,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -907,7 +1243,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -927,7 +1263,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -943,11 +1279,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -965,6 +1301,786 @@
       </c>
       <c r="F5" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" t="s">
+        <v>152</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" t="s">
+        <v>176</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>179</v>
+      </c>
+      <c r="B40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" t="s">
+        <v>181</v>
+      </c>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>182</v>
+      </c>
+      <c r="B41" t="s">
+        <v>183</v>
+      </c>
+      <c r="C41" t="s">
+        <v>184</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>185</v>
+      </c>
+      <c r="B42" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" t="s">
+        <v>187</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" t="s">
+        <v>192</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" t="s">
+        <v>193</v>
+      </c>
+      <c r="F44" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1135,7 +2251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D883BCCB-1427-F54B-B447-B53E8EA23A3A}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>

</xml_diff>

<commit_message>
added Wednesday speeches from Cision
</commit_message>
<xml_diff>
--- a/DNC/dnc.metadata.xlsx
+++ b/DNC/dnc.metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/DNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F9E79A-274C-1B42-A737-5B7D0D41BD82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087D33AD-3AB0-694C-A6CB-9304D923AA5B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="1" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="2" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="312">
   <si>
     <t>Last</t>
   </si>
@@ -628,6 +628,348 @@
   </si>
   <si>
     <t>dnc.byron.txt</t>
+  </si>
+  <si>
+    <t>Driffin</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>dnc.driffin.txt</t>
+  </si>
+  <si>
+    <t>Tanden</t>
+  </si>
+  <si>
+    <t>Neera</t>
+  </si>
+  <si>
+    <t>dnc.tanden.txt</t>
+  </si>
+  <si>
+    <t>Grisham</t>
+  </si>
+  <si>
+    <t>dnc.grisham.txt</t>
+  </si>
+  <si>
+    <t>Norton</t>
+  </si>
+  <si>
+    <t>Eleanor</t>
+  </si>
+  <si>
+    <t>dnc.norton.txt</t>
+  </si>
+  <si>
+    <t>Schiff</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>dnc.schiff.txt</t>
+  </si>
+  <si>
+    <t>Waters</t>
+  </si>
+  <si>
+    <t>Maxine</t>
+  </si>
+  <si>
+    <t>dnc.waters.txt</t>
+  </si>
+  <si>
+    <t>Hogue</t>
+  </si>
+  <si>
+    <t>Ilyse</t>
+  </si>
+  <si>
+    <t>dnc.hogue.txt</t>
+  </si>
+  <si>
+    <t>Gillum</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>dnc.gillum.txt</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Caucus</t>
+  </si>
+  <si>
+    <t>dnc.asian.txt</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>Brooks</t>
+  </si>
+  <si>
+    <t>dnc.bellbrooks.txt</t>
+  </si>
+  <si>
+    <t>deBlasio</t>
+  </si>
+  <si>
+    <t>dnc.deblasio.txt</t>
+  </si>
+  <si>
+    <t>Grubbe</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>dnc.grubbe.txt</t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>dnc.jacksonjesse.txt</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>dnc.jonesstar.txt</t>
+  </si>
+  <si>
+    <t>Weaver</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>dnc.weaver.txt</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>dnc.blackcaucus.txt</t>
+  </si>
+  <si>
+    <t>Schriock</t>
+  </si>
+  <si>
+    <t>tephanie</t>
+  </si>
+  <si>
+    <t>dnc.schriock.txt</t>
+  </si>
+  <si>
+    <t>Reid</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>dnc.reidharry.txt</t>
+  </si>
+  <si>
+    <t>Dorff</t>
+  </si>
+  <si>
+    <t>jamie</t>
+  </si>
+  <si>
+    <t>dnc.dorff.txt</t>
+  </si>
+  <si>
+    <t>Belkofer</t>
+  </si>
+  <si>
+    <t>Sharon</t>
+  </si>
+  <si>
+    <t>dnc.belkofer.txt</t>
+  </si>
+  <si>
+    <t>Salguero</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>dnc.salguero.txt</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Shelia</t>
+  </si>
+  <si>
+    <t>dnc.leeshelia.txt</t>
+  </si>
+  <si>
+    <t>Duggan</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>dnc.duggan.txt</t>
+  </si>
+  <si>
+    <t>Omalley</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>dnc.omalley.txt</t>
+  </si>
+  <si>
+    <t>Sigourney</t>
+  </si>
+  <si>
+    <t>dnc.weaversigourney.txt</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>dnc.brownjerry.txt</t>
+  </si>
+  <si>
+    <t>Daniels</t>
+  </si>
+  <si>
+    <t>dnc.danielslee.txt</t>
+  </si>
+  <si>
+    <t>Murphy</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>dnc.murphychris.txt</t>
+  </si>
+  <si>
+    <t>Ramsey</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>dnc.ramsey.txt</t>
+  </si>
+  <si>
+    <t>Bassett</t>
+  </si>
+  <si>
+    <t>Angela</t>
+  </si>
+  <si>
+    <t>dnc.bassett.txt</t>
+  </si>
+  <si>
+    <t>Felicia</t>
+  </si>
+  <si>
+    <t>dnc.sandersfelicia.txt</t>
+  </si>
+  <si>
+    <t>Sheppard</t>
+  </si>
+  <si>
+    <t>polly</t>
+  </si>
+  <si>
+    <t>dnc.sheppard.txt</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>dnc.kellymark.txt</t>
+  </si>
+  <si>
+    <t>Hutson</t>
+  </si>
+  <si>
+    <t>dnc.hutson.txt</t>
+  </si>
+  <si>
+    <t>Kavanaugh</t>
+  </si>
+  <si>
+    <t>Kristen</t>
+  </si>
+  <si>
+    <t>dnc.kavanaugh.txt</t>
+  </si>
+  <si>
+    <t>Panetta</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>dnc.panetta.txt</t>
+  </si>
+  <si>
+    <t>Lujan</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>dnc.lujan.txt</t>
+  </si>
+  <si>
+    <t>Smegielski</t>
+  </si>
+  <si>
+    <t>dnc.smegielski.txt</t>
+  </si>
+  <si>
+    <t>Erica</t>
+  </si>
+  <si>
+    <t>Reed</t>
+  </si>
+  <si>
+    <t>Kasim</t>
+  </si>
+  <si>
+    <t>dnc.reedkasim.txt</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>dnc.scottbobby.txt</t>
+  </si>
+  <si>
+    <t>Our</t>
+  </si>
+  <si>
+    <t>dnc.ouramerica.txt</t>
   </si>
 </sst>
 </file>
@@ -1202,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B00C89-5F5B-B54D-834C-45D0C98C9369}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -2099,11 +2441,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C4212-161F-404C-AC20-375466C438FF}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2268,6 +2610,826 @@
         <v>193</v>
       </c>
       <c r="F8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C21" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>234</v>
+      </c>
+      <c r="B22" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" t="s">
+        <v>236</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" t="s">
+        <v>239</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" t="s">
+        <v>241</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>242</v>
+      </c>
+      <c r="B25" t="s">
+        <v>243</v>
+      </c>
+      <c r="C25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C26" t="s">
+        <v>247</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>248</v>
+      </c>
+      <c r="B27" t="s">
+        <v>249</v>
+      </c>
+      <c r="C27" t="s">
+        <v>250</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>251</v>
+      </c>
+      <c r="B28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28" t="s">
+        <v>253</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>254</v>
+      </c>
+      <c r="B29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" t="s">
+        <v>256</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>257</v>
+      </c>
+      <c r="B30" t="s">
+        <v>258</v>
+      </c>
+      <c r="C30" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31" t="s">
+        <v>261</v>
+      </c>
+      <c r="C31" t="s">
+        <v>262</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>263</v>
+      </c>
+      <c r="B32" t="s">
+        <v>264</v>
+      </c>
+      <c r="C32" t="s">
+        <v>265</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>237</v>
+      </c>
+      <c r="B33" t="s">
+        <v>266</v>
+      </c>
+      <c r="C33" t="s">
+        <v>267</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>268</v>
+      </c>
+      <c r="B34" t="s">
+        <v>269</v>
+      </c>
+      <c r="C34" t="s">
+        <v>270</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>271</v>
+      </c>
+      <c r="B35" t="s">
+        <v>257</v>
+      </c>
+      <c r="C35" t="s">
+        <v>272</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>273</v>
+      </c>
+      <c r="B36" t="s">
+        <v>274</v>
+      </c>
+      <c r="C36" t="s">
+        <v>275</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>276</v>
+      </c>
+      <c r="B37" t="s">
+        <v>277</v>
+      </c>
+      <c r="C37" t="s">
+        <v>278</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>279</v>
+      </c>
+      <c r="B38" t="s">
+        <v>280</v>
+      </c>
+      <c r="C38" t="s">
+        <v>281</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>282</v>
+      </c>
+      <c r="C39" t="s">
+        <v>283</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>284</v>
+      </c>
+      <c r="B40" t="s">
+        <v>285</v>
+      </c>
+      <c r="C40" t="s">
+        <v>286</v>
+      </c>
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>287</v>
+      </c>
+      <c r="B41" t="s">
+        <v>288</v>
+      </c>
+      <c r="C41" t="s">
+        <v>289</v>
+      </c>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>290</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>291</v>
+      </c>
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>292</v>
+      </c>
+      <c r="B43" t="s">
+        <v>293</v>
+      </c>
+      <c r="C43" t="s">
+        <v>294</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>295</v>
+      </c>
+      <c r="B44" t="s">
+        <v>296</v>
+      </c>
+      <c r="C44" t="s">
+        <v>297</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>298</v>
+      </c>
+      <c r="B45" t="s">
+        <v>299</v>
+      </c>
+      <c r="C45" t="s">
+        <v>300</v>
+      </c>
+      <c r="D45" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>301</v>
+      </c>
+      <c r="B46" t="s">
+        <v>303</v>
+      </c>
+      <c r="C46" t="s">
+        <v>302</v>
+      </c>
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>304</v>
+      </c>
+      <c r="B47" t="s">
+        <v>305</v>
+      </c>
+      <c r="C47" t="s">
+        <v>306</v>
+      </c>
+      <c r="D47" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>307</v>
+      </c>
+      <c r="B48" t="s">
+        <v>308</v>
+      </c>
+      <c r="C48" t="s">
+        <v>309</v>
+      </c>
+      <c r="D48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" t="s">
+        <v>310</v>
+      </c>
+      <c r="C49" t="s">
+        <v>311</v>
+      </c>
+      <c r="D49" t="s">
+        <v>53</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Thursday Speeches from Cision
</commit_message>
<xml_diff>
--- a/DNC/dnc.metadata.xlsx
+++ b/DNC/dnc.metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/DNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087D33AD-3AB0-694C-A6CB-9304D923AA5B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5536935B-78BE-BC43-9A95-3F69446818D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="2" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="3" xr2:uid="{3C073B89-2240-F743-BE85-AA35D6D2EF38}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="450">
   <si>
     <t>Last</t>
   </si>
@@ -970,6 +970,420 @@
   </si>
   <si>
     <t>dnc.ouramerica.txt</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>Bernice</t>
+  </si>
+  <si>
+    <t>dnc.kingb.txt</t>
+  </si>
+  <si>
+    <t>Torres</t>
+  </si>
+  <si>
+    <t>Eddie</t>
+  </si>
+  <si>
+    <t>dnc.torres.txt</t>
+  </si>
+  <si>
+    <t>Karpinski</t>
+  </si>
+  <si>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>dnc.karpinski.txt</t>
+  </si>
+  <si>
+    <t>Flanagan</t>
+  </si>
+  <si>
+    <t>Peggy</t>
+  </si>
+  <si>
+    <t>dnc.flanagan.txt</t>
+  </si>
+  <si>
+    <t>Deutch</t>
+  </si>
+  <si>
+    <t>Ted</t>
+  </si>
+  <si>
+    <t>dnc.deutch.txt</t>
+  </si>
+  <si>
+    <t>Sellers</t>
+  </si>
+  <si>
+    <t>Bakari</t>
+  </si>
+  <si>
+    <t>dnc.sellers.txt</t>
+  </si>
+  <si>
+    <t>Harrison</t>
+  </si>
+  <si>
+    <t>Jamie</t>
+  </si>
+  <si>
+    <t>dnc.harrisonjamie.txt</t>
+  </si>
+  <si>
+    <t>Griffin</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>dnc.griffinchad.txt</t>
+  </si>
+  <si>
+    <t>Duran</t>
+  </si>
+  <si>
+    <t>Crisanta</t>
+  </si>
+  <si>
+    <t>dnc.duran.txt</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>Cedric</t>
+  </si>
+  <si>
+    <t>dnc.richmondc.txt</t>
+  </si>
+  <si>
+    <t>Akbari</t>
+  </si>
+  <si>
+    <t>Raumesh</t>
+  </si>
+  <si>
+    <t>dnc.akbari.txt</t>
+  </si>
+  <si>
+    <t>Cleaver</t>
+  </si>
+  <si>
+    <t>Emanuel</t>
+  </si>
+  <si>
+    <t>dnc.cleaver.txt</t>
+  </si>
+  <si>
+    <t>Maloney</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>dnc.maloney.txt</t>
+  </si>
+  <si>
+    <t>Demetrios</t>
+  </si>
+  <si>
+    <t>Archbishop</t>
+  </si>
+  <si>
+    <t>dnc.demetrios.txt</t>
+  </si>
+  <si>
+    <t>McBride</t>
+  </si>
+  <si>
+    <t>dnc.mcbride.txt</t>
+  </si>
+  <si>
+    <t>Beatty</t>
+  </si>
+  <si>
+    <t>Joyce</t>
+  </si>
+  <si>
+    <t>dnc.beatty.txt</t>
+  </si>
+  <si>
+    <t>Garcetti</t>
+  </si>
+  <si>
+    <t>dnc.garcetti.txt</t>
+  </si>
+  <si>
+    <t>Dayton</t>
+  </si>
+  <si>
+    <t>dnc.dayton.txt</t>
+  </si>
+  <si>
+    <t>McGinty</t>
+  </si>
+  <si>
+    <t>Katie</t>
+  </si>
+  <si>
+    <t>dnc.mcginty.txt</t>
+  </si>
+  <si>
+    <t>Durckworth</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>dnc.duckworth.txt</t>
+  </si>
+  <si>
+    <t>Clyburn</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>dnc.clyburn.txt</t>
+  </si>
+  <si>
+    <t>Senate</t>
+  </si>
+  <si>
+    <t>dnc.senatewomen.txt</t>
+  </si>
+  <si>
+    <t>Nutter</t>
+  </si>
+  <si>
+    <t>dnc.nutter.txt</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>Marlon</t>
+  </si>
+  <si>
+    <t>dnc.marshallmarlon.txt</t>
+  </si>
+  <si>
+    <t>Kihuen</t>
+  </si>
+  <si>
+    <t>Ruben</t>
+  </si>
+  <si>
+    <t>dnc.kihuen.txt</t>
+  </si>
+  <si>
+    <t>Praeli</t>
+  </si>
+  <si>
+    <t>Lorella</t>
+  </si>
+  <si>
+    <t>dnc.praeli.txt</t>
+  </si>
+  <si>
+    <t>Castro</t>
+  </si>
+  <si>
+    <t>Joaquin</t>
+  </si>
+  <si>
+    <t>dnc.castroj.txt</t>
+  </si>
+  <si>
+    <t>Huerta</t>
+  </si>
+  <si>
+    <t>Dolores</t>
+  </si>
+  <si>
+    <t>dnc.huerta.txt</t>
+  </si>
+  <si>
+    <t>Cuomo</t>
+  </si>
+  <si>
+    <t>dnc.cuomo.txt</t>
+  </si>
+  <si>
+    <t>Pelosi</t>
+  </si>
+  <si>
+    <t>Nancy</t>
+  </si>
+  <si>
+    <t>dnc.pelosin.txt</t>
+  </si>
+  <si>
+    <t>dnc.ryantim.txt</t>
+  </si>
+  <si>
+    <t>Hickenlooper</t>
+  </si>
+  <si>
+    <t>dnc.hickenlooper.txt</t>
+  </si>
+  <si>
+    <t>Ivey</t>
+  </si>
+  <si>
+    <t>Steenburgen</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>dnc.maryted.txt</t>
+  </si>
+  <si>
+    <t>Henrietta</t>
+  </si>
+  <si>
+    <t>dnc.ivey.txt</t>
+  </si>
+  <si>
+    <t>Wils</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>dnc.wils.txt</t>
+  </si>
+  <si>
+    <t>Mathias</t>
+  </si>
+  <si>
+    <t>Beth</t>
+  </si>
+  <si>
+    <t>dnc.mathias.txt</t>
+  </si>
+  <si>
+    <t>Walcott</t>
+  </si>
+  <si>
+    <t>Jansen</t>
+  </si>
+  <si>
+    <t>dnc.jensenjake.txt</t>
+  </si>
+  <si>
+    <t>Granholm</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>dnc.granholm.txt</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>dnc.wolftom.txt</t>
+  </si>
+  <si>
+    <t>Elmets</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>dnc.elmets.txt</t>
+  </si>
+  <si>
+    <t>Lim</t>
+  </si>
+  <si>
+    <t>dnc.lim.txt</t>
+  </si>
+  <si>
+    <t>Valdez</t>
+  </si>
+  <si>
+    <t>Lupe</t>
+  </si>
+  <si>
+    <t>dnc.valdezlupe.txt</t>
+  </si>
+  <si>
+    <t>Abdul-Jabbar</t>
+  </si>
+  <si>
+    <t>Kareem</t>
+  </si>
+  <si>
+    <t>dnc.jabbar.txt</t>
+  </si>
+  <si>
+    <t>Lieu</t>
+  </si>
+  <si>
+    <t>dnc.lieu.txt</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>dnc.allenjohn.txt</t>
+  </si>
+  <si>
+    <t>Groberg</t>
+  </si>
+  <si>
+    <t>Florent</t>
+  </si>
+  <si>
+    <t>dnc.groberg.txt</t>
+  </si>
+  <si>
+    <t>Moretz</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>dnc.moretz.txt</t>
+  </si>
+  <si>
+    <t>Sherrod</t>
+  </si>
+  <si>
+    <t>dnc.browns.txt</t>
+  </si>
+  <si>
+    <t>Becerra</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>dnc.becerra.txt</t>
+  </si>
+  <si>
+    <t>Perry</t>
+  </si>
+  <si>
+    <t>Katy</t>
+  </si>
+  <si>
+    <t>dnc.perryk.txt</t>
+  </si>
+  <si>
+    <t>Shillady</t>
+  </si>
+  <si>
+    <t>dnc.shillady.txt</t>
   </si>
 </sst>
 </file>
@@ -2443,9 +2857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C4212-161F-404C-AC20-375466C438FF}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3440,16 +3854,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D883BCCB-1427-F54B-B447-B53E8EA23A3A}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -3532,6 +3947,1026 @@
         <v>82</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" t="s">
+        <v>323</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>324</v>
+      </c>
+      <c r="B9" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" t="s">
+        <v>326</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B10" t="s">
+        <v>328</v>
+      </c>
+      <c r="C10" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B12" t="s">
+        <v>334</v>
+      </c>
+      <c r="C12" t="s">
+        <v>335</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>336</v>
+      </c>
+      <c r="B13" t="s">
+        <v>337</v>
+      </c>
+      <c r="C13" t="s">
+        <v>338</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" t="s">
+        <v>340</v>
+      </c>
+      <c r="C14" t="s">
+        <v>341</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>342</v>
+      </c>
+      <c r="B15" t="s">
+        <v>343</v>
+      </c>
+      <c r="C15" t="s">
+        <v>344</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>345</v>
+      </c>
+      <c r="B16" t="s">
+        <v>346</v>
+      </c>
+      <c r="C16" t="s">
+        <v>347</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" t="s">
+        <v>349</v>
+      </c>
+      <c r="C17" t="s">
+        <v>350</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>351</v>
+      </c>
+      <c r="B18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C18" t="s">
+        <v>353</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>193</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>355</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>356</v>
+      </c>
+      <c r="B20" t="s">
+        <v>357</v>
+      </c>
+      <c r="C20" t="s">
+        <v>358</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>359</v>
+      </c>
+      <c r="B21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" t="s">
+        <v>360</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>361</v>
+      </c>
+      <c r="B22" t="s">
+        <v>288</v>
+      </c>
+      <c r="C22" t="s">
+        <v>362</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>363</v>
+      </c>
+      <c r="B23" t="s">
+        <v>364</v>
+      </c>
+      <c r="C23" t="s">
+        <v>365</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>366</v>
+      </c>
+      <c r="B24" t="s">
+        <v>367</v>
+      </c>
+      <c r="C24" t="s">
+        <v>368</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>369</v>
+      </c>
+      <c r="B25" t="s">
+        <v>370</v>
+      </c>
+      <c r="C25" t="s">
+        <v>371</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>372</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>373</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>374</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>375</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>376</v>
+      </c>
+      <c r="B28" t="s">
+        <v>377</v>
+      </c>
+      <c r="C28" t="s">
+        <v>378</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>379</v>
+      </c>
+      <c r="B29" t="s">
+        <v>380</v>
+      </c>
+      <c r="C29" t="s">
+        <v>381</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>382</v>
+      </c>
+      <c r="B30" t="s">
+        <v>383</v>
+      </c>
+      <c r="C30" t="s">
+        <v>384</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>385</v>
+      </c>
+      <c r="B31" t="s">
+        <v>386</v>
+      </c>
+      <c r="C31" t="s">
+        <v>387</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>388</v>
+      </c>
+      <c r="B32" t="s">
+        <v>389</v>
+      </c>
+      <c r="C32" t="s">
+        <v>390</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>391</v>
+      </c>
+      <c r="B33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" t="s">
+        <v>392</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>393</v>
+      </c>
+      <c r="B34" t="s">
+        <v>394</v>
+      </c>
+      <c r="C34" t="s">
+        <v>395</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" t="s">
+        <v>396</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>397</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>398</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>399</v>
+      </c>
+      <c r="B37" t="s">
+        <v>403</v>
+      </c>
+      <c r="C37" t="s">
+        <v>404</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>400</v>
+      </c>
+      <c r="B38" t="s">
+        <v>401</v>
+      </c>
+      <c r="C38" t="s">
+        <v>402</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>405</v>
+      </c>
+      <c r="B39" t="s">
+        <v>406</v>
+      </c>
+      <c r="C39" t="s">
+        <v>407</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>408</v>
+      </c>
+      <c r="B40" t="s">
+        <v>409</v>
+      </c>
+      <c r="C40" t="s">
+        <v>410</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B41" t="s">
+        <v>412</v>
+      </c>
+      <c r="C41" t="s">
+        <v>413</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>414</v>
+      </c>
+      <c r="B42" t="s">
+        <v>415</v>
+      </c>
+      <c r="C42" t="s">
+        <v>416</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>417</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" t="s">
+        <v>418</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>419</v>
+      </c>
+      <c r="B44" t="s">
+        <v>420</v>
+      </c>
+      <c r="C44" t="s">
+        <v>421</v>
+      </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>422</v>
+      </c>
+      <c r="B45" t="s">
+        <v>415</v>
+      </c>
+      <c r="C45" t="s">
+        <v>423</v>
+      </c>
+      <c r="D45" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>424</v>
+      </c>
+      <c r="B46" t="s">
+        <v>425</v>
+      </c>
+      <c r="C46" t="s">
+        <v>426</v>
+      </c>
+      <c r="D46" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>427</v>
+      </c>
+      <c r="B47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C47" t="s">
+        <v>429</v>
+      </c>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>430</v>
+      </c>
+      <c r="B48" t="s">
+        <v>325</v>
+      </c>
+      <c r="C48" t="s">
+        <v>431</v>
+      </c>
+      <c r="D48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>432</v>
+      </c>
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" t="s">
+        <v>433</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>434</v>
+      </c>
+      <c r="B50" t="s">
+        <v>435</v>
+      </c>
+      <c r="C50" t="s">
+        <v>436</v>
+      </c>
+      <c r="D50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>437</v>
+      </c>
+      <c r="B51" t="s">
+        <v>438</v>
+      </c>
+      <c r="C51" t="s">
+        <v>439</v>
+      </c>
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>268</v>
+      </c>
+      <c r="B52" t="s">
+        <v>440</v>
+      </c>
+      <c r="C52" t="s">
+        <v>441</v>
+      </c>
+      <c r="D52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>442</v>
+      </c>
+      <c r="B53" t="s">
+        <v>443</v>
+      </c>
+      <c r="C53" t="s">
+        <v>444</v>
+      </c>
+      <c r="D53" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>445</v>
+      </c>
+      <c r="B54" t="s">
+        <v>446</v>
+      </c>
+      <c r="C54" t="s">
+        <v>447</v>
+      </c>
+      <c r="D54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>448</v>
+      </c>
+      <c r="B55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" t="s">
+        <v>449</v>
+      </c>
+      <c r="D55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" t="s">
+        <v>193</v>
+      </c>
+      <c r="F55" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>